<commit_message>
Agregar generación de contraseña
En el panel de admin, al crear una empresa, la contraseña se genera automáticamente.
</commit_message>
<xml_diff>
--- a/lib/data/ListaEmpresa.xlsx
+++ b/lib/data/ListaEmpresa.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -2551,9 +2551,35 @@
         <v>MB7047612024</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84">
+        <v>705</v>
+      </c>
+      <c r="B84" t="str">
+        <v>123</v>
+      </c>
+      <c r="C84" t="str">
+        <v>Anglo</v>
+      </c>
+      <c r="D84" t="str">
+        <v>Si</v>
+      </c>
+      <c r="E84" t="str">
+        <v>yo</v>
+      </c>
+      <c r="F84" t="str">
+        <v>anglo@prueba.com</v>
+      </c>
+      <c r="G84" t="str">
+        <v>1231234</v>
+      </c>
+      <c r="H84" t="str">
+        <v>jajajaja</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H83"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H84"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Habilitar la edición de los campos de las tablas
</commit_message>
<xml_diff>
--- a/lib/data/ListaEmpresa.xlsx
+++ b/lib/data/ListaEmpresa.xlsx
@@ -399,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -2559,16 +2559,16 @@
         <v>123</v>
       </c>
       <c r="C84" t="str">
-        <v>Anglo</v>
+        <v>Anglo TEST</v>
       </c>
       <c r="D84" t="str">
-        <v>Si</v>
+        <v>Si pero ahora no</v>
       </c>
       <c r="E84" t="str">
         <v>yo</v>
       </c>
       <c r="F84" t="str">
-        <v>anglo@prueba.com</v>
+        <v>anglo@prueba.cl</v>
       </c>
       <c r="G84" t="str">
         <v>1231234</v>

</xml_diff>